<commit_message>
update course excel files
</commit_message>
<xml_diff>
--- a/courses/excel/offshore/SEAPAE/aibt/ACE_AVIATION_AEROSPACE_ACADEMY.xlsx
+++ b/courses/excel/offshore/SEAPAE/aibt/ACE_AVIATION_AEROSPACE_ACADEMY.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aibtaus-my.sharepoint.com/personal/f_zhang_aibtglobal_edu_au/Documents/App for VC/excel table template/courses/courses/excel/offshore/SEAPAE/aibt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelon\Documents\Code\ViskeeConsultancy\Viskee-Consultancy-Configuration\courses\excel\offshore\SEAPAE\aibt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_C72790AC758F7B96A37496758E9FA223E7E6BADC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7EE668E-7909-45FC-8ED6-FAA02EE5D3F4}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18345" yWindow="-16320" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>vetCode</t>
   </si>
@@ -89,9 +88,6 @@
     <t>AVI50119</t>
   </si>
   <si>
-    <t>ACE AVIATION</t>
-  </si>
-  <si>
     <t>Diploma of Aviation (Aviation Management)</t>
   </si>
   <si>
@@ -101,24 +97,24 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Promotion valid until  31th Dec 2021</t>
-  </si>
-  <si>
     <t>0101215</t>
   </si>
   <si>
     <t>12,500 tuition fee + 200 handling fee</t>
+  </si>
+  <si>
+    <t>AVIATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -126,13 +122,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -450,35 +446,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.625" customWidth="1"/>
+    <col min="5" max="5" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,18 +530,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="45">
+    <row r="2" spans="1:18" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="E2" s="2">
         <v>52</v>
@@ -553,26 +549,24 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2" s="3">
         <v>12500</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="R2" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>